<commit_message>
Revert "removed the breakpoint"
This reverts commit 26fae2c044e3d2981031dddd65f3a65e3f6edb53.
</commit_message>
<xml_diff>
--- a/TestData/Administration_Input_File.xlsx
+++ b/TestData/Administration_Input_File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ustiws02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA86A089-721A-4951-AF73-92A61DF43CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962A053F-9F4D-4DB4-9BED-A97E5E8820D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -66,18 +66,6 @@
   </si>
   <si>
     <t>CANADA,INDIA,PERU,USA</t>
-  </si>
-  <si>
-    <t>Shyam Tiwari</t>
-  </si>
-  <si>
-    <t>shyam.tiwari@ingrammicro.com</t>
-  </si>
-  <si>
-    <t>Sales Associate - Basic+,Finance Associate - Basic+</t>
-  </si>
-  <si>
-    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -173,9 +161,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -501,7 +492,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,19 +505,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -534,42 +525,28 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{4736C6A0-287B-4B22-9FB5-E6FC3E451EEC}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{7AB5D68E-EA9B-4778-9AA9-9F4001304ECC}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{92A10752-3887-4586-BC37-5EBE1A9D03F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>